<commit_message>
Added leases. Also cleaned up some code. Started trying to port to .Net core, but there are some issues to resolve around the messaging.
</commit_message>
<xml_diff>
--- a/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Product Pricers/PropertyPricer.xlsx
+++ b/FpML.V5r3.Applications/ExcelAPI/Spreadsheets/Product Pricers/PropertyPricer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\Documents\Visual Studio 2019\Projects\Highlander\FpML.V5r3.Applications\ExcelAPI\Spreadsheets\Product Pricers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8369082-06A2-4C86-8BD7-1C4B56045813}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{202B76FB-781D-4FFF-A76E-72CF9D2F6E4B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1230" yWindow="0" windowWidth="26370" windowHeight="14820" tabRatio="568" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="465" windowWidth="26370" windowHeight="14820" tabRatio="568" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PropertyData" sheetId="11" r:id="rId1"/>
@@ -2372,7 +2372,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="107">
   <si>
     <t>NAB</t>
   </si>
@@ -2650,9 +2650,6 @@
     <t>IsParty1Tenant</t>
   </si>
   <si>
-    <t>Commercial.Sydney.CBD.George.1</t>
-  </si>
-  <si>
     <t>AMP</t>
   </si>
   <si>
@@ -2684,6 +2681,18 @@
   </si>
   <si>
     <t>sqm</t>
+  </si>
+  <si>
+    <t>Postcode</t>
+  </si>
+  <si>
+    <t>LeaseTransaction</t>
+  </si>
+  <si>
+    <t>leaseTransaction</t>
+  </si>
+  <si>
+    <t>test_002</t>
   </si>
 </sst>
 </file>
@@ -4072,10 +4081,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4086,18 +4095,19 @@
     <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="42.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="20.25">
+    <row r="1" spans="1:17" ht="20.25">
       <c r="A1" s="33" t="s">
         <v>51</v>
       </c>
@@ -4117,37 +4127,40 @@
         <v>61</v>
       </c>
       <c r="G1" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="H1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="P1" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="P1" s="34" t="s">
+      <c r="Q1" s="34" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -4166,39 +4179,42 @@
       <c r="F2" t="s">
         <v>64</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2">
+        <v>2025</v>
+      </c>
+      <c r="H2" t="s">
         <v>65</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>66</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>10</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>6</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>22</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="O2" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="O2" s="9" t="s">
+      <c r="P2" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="P2" t="str">
-        <f>_xll.HLV5r3.Financial.Cache.CreateProperty(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N1:O1,N2:O2)</f>
+      <c r="Q2" t="str">
+        <f>_xll.HLV5r3.Financial.Cache.CreateProperty(A2,B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O1:P1,O2:P2)</f>
         <v>Residential.Sydney.Woollahra.Jersey.AlexHouse</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>83</v>
       </c>
@@ -4217,35 +4233,38 @@
       <c r="F3" t="s">
         <v>64</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>2025</v>
+      </c>
+      <c r="H3" t="s">
         <v>65</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>66</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>10</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>6</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>5</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>87</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="P3" t="str">
-        <f>_xll.HLV5r3.Financial.Cache.CreateProperty(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N2:O2,N3:O3)</f>
+      <c r="Q3" t="str">
+        <f>_xll.HLV5r3.Financial.Cache.CreateProperty(A3,B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O2:P2,O3:P3)</f>
         <v>Commercial.Sydney.CBD.George.1</v>
       </c>
     </row>
@@ -4257,10 +4276,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{161306B7-A8C5-4EA0-B5E9-3CA5B90DB89A}">
-  <dimension ref="A1:P29"/>
+  <dimension ref="A1:P55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4447,7 +4466,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>77</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:16">
@@ -4455,7 +4474,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>78</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:16">
@@ -4464,20 +4483,20 @@
       </c>
       <c r="D8" s="2">
         <f ca="1">D18</f>
-        <v>43680</v>
+        <v>43721</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="C9" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>97</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="C10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D10">
         <v>100</v>
@@ -4485,24 +4504,24 @@
     </row>
     <row r="11" spans="1:16">
       <c r="C11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="C12" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D12" s="2">
         <f ca="1">D19+365</f>
-        <v>44048</v>
+        <v>44089</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="C13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D13" s="37">
         <v>0.03</v>
@@ -4538,7 +4557,7 @@
       </c>
       <c r="D18" s="2">
         <f ca="1">TODAY()</f>
-        <v>43680</v>
+        <v>43721</v>
       </c>
     </row>
     <row r="19" spans="3:4">
@@ -4547,7 +4566,7 @@
       </c>
       <c r="D19" s="2">
         <f ca="1">D18+3</f>
-        <v>43683</v>
+        <v>43724</v>
       </c>
     </row>
     <row r="20" spans="3:4">
@@ -4587,20 +4606,21 @@
         <v>2</v>
       </c>
       <c r="D24" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="3:4">
       <c r="C25" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
+      </c>
+      <c r="D25" s="9" t="str">
+        <f>P3</f>
+        <v>Commercial.Sydney.CBD.George.1</v>
       </c>
     </row>
     <row r="26" spans="3:4">
       <c r="C26" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="27" spans="3:4">
@@ -4608,13 +4628,197 @@
         <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="3:4">
       <c r="C29" s="1" t="str">
         <f ca="1">_xll.HLV5r3.Financial.Cache.CreateLeaseTradeWithProperties(D21,D20,D23,D24,D18,D19,D15,D16,D17,D22,D26,D25,D27,C5:D13)</f>
         <v>Trade.SpreadSheet.leaseTransaction.test_001</v>
+      </c>
+    </row>
+    <row r="31" spans="3:4">
+      <c r="C31" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" s="36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="3:4">
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="3:4">
+      <c r="C33" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4">
+      <c r="C34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="2">
+        <f ca="1">D44</f>
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4">
+      <c r="C35" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4">
+      <c r="C36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="3:4">
+      <c r="C37" t="s">
+        <v>99</v>
+      </c>
+      <c r="D37" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="38" spans="3:4">
+      <c r="C38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D38" s="2">
+        <f ca="1">D45+365</f>
+        <v>44089</v>
+      </c>
+    </row>
+    <row r="39" spans="3:4">
+      <c r="C39" t="s">
+        <v>101</v>
+      </c>
+      <c r="D39" s="37">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4">
+      <c r="C41" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="3:4">
+      <c r="C42" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="43" spans="3:4">
+      <c r="C43" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="D43" s="25">
+        <v>15000000</v>
+      </c>
+    </row>
+    <row r="44" spans="3:4">
+      <c r="C44" t="s">
+        <v>1</v>
+      </c>
+      <c r="D44" s="2">
+        <f ca="1">TODAY()</f>
+        <v>43721</v>
+      </c>
+    </row>
+    <row r="45" spans="3:4">
+      <c r="C45" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D45" s="2">
+        <f ca="1">D44+3</f>
+        <v>43724</v>
+      </c>
+    </row>
+    <row r="46" spans="3:4">
+      <c r="C46" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="3:4">
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="48" spans="3:4">
+      <c r="C48" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4">
+      <c r="C49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="C50" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="3:4">
+      <c r="C51" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" s="9" t="str">
+        <f>P2</f>
+        <v>Residential.Sydney.Woollahra.Jersey.AlexHouse</v>
+      </c>
+    </row>
+    <row r="52" spans="3:4">
+      <c r="C52" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4">
+      <c r="C53" t="s">
+        <v>70</v>
+      </c>
+      <c r="D53" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="55" spans="3:4">
+      <c r="C55" s="1" t="str">
+        <f ca="1">_xll.HLV5r3.Financial.Cache.CreateLeaseTrade(D47,D46,D49,D50,D44,D45,D41,D42,D43,D48,D52,D51,D53)</f>
+        <v>Trade.SpreadSheet.leaseTransaction.test_002</v>
       </c>
     </row>
   </sheetData>
@@ -4628,7 +4832,7 @@
   <dimension ref="B1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -4740,7 +4944,7 @@
       </c>
       <c r="C10" s="2">
         <f ca="1">TODAY()</f>
-        <v>43680</v>
+        <v>43721</v>
       </c>
       <c r="H10" t="e">
         <f ca="1"/>
@@ -4753,7 +4957,7 @@
       </c>
       <c r="C11" s="2">
         <f ca="1">C10+3</f>
-        <v>43683</v>
+        <v>43724</v>
       </c>
       <c r="H11" t="e">
         <f ca="1"/>
@@ -4816,7 +5020,7 @@
       </c>
       <c r="C16" s="2">
         <f ca="1">C10</f>
-        <v>43680</v>
+        <v>43721</v>
       </c>
       <c r="E16" t="e">
         <f t="array" aca="1" ref="E16:F22" ca="1">_xll.HLV5r3.Financial.Cache.ViewValuationReport(E12)</f>
@@ -4876,7 +5080,7 @@
         <v>82</v>
       </c>
       <c r="C20" s="9" t="str">
-        <f>PropertyData!P3</f>
+        <f>PropertyData!Q3</f>
         <v>Commercial.Sydney.CBD.George.1</v>
       </c>
       <c r="E20" t="e">
@@ -5188,7 +5392,7 @@
       </c>
       <c r="K2" s="15">
         <f ca="1">TODAY()</f>
-        <v>43680</v>
+        <v>43721</v>
       </c>
       <c r="L2" s="32"/>
       <c r="N2" s="5" t="s">
@@ -5301,11 +5505,11 @@
       </c>
       <c r="F7" s="2">
         <f ca="1">TODAY()-20</f>
-        <v>43660</v>
+        <v>43701</v>
       </c>
       <c r="G7" s="2">
         <f ca="1">F7+3</f>
-        <v>43663</v>
+        <v>43704</v>
       </c>
       <c r="H7" s="8">
         <v>100</v>
@@ -5383,11 +5587,11 @@
       </c>
       <c r="F9" s="2">
         <f ca="1">F7+2</f>
-        <v>43662</v>
+        <v>43703</v>
       </c>
       <c r="G9" s="2">
         <f ca="1">F9+3</f>
-        <v>43665</v>
+        <v>43706</v>
       </c>
       <c r="H9" s="8">
         <f>H7+20</f>
@@ -5475,11 +5679,11 @@
       </c>
       <c r="F11" s="2">
         <f ca="1">F9+2</f>
-        <v>43664</v>
+        <v>43705</v>
       </c>
       <c r="G11" s="2">
         <f ca="1">F11+3</f>
-        <v>43667</v>
+        <v>43708</v>
       </c>
       <c r="H11" s="8">
         <f>H9+20</f>
@@ -5567,11 +5771,11 @@
       </c>
       <c r="F13" s="2">
         <f ca="1">F11+2</f>
-        <v>43666</v>
+        <v>43707</v>
       </c>
       <c r="G13" s="2">
         <f ca="1">F13+3</f>
-        <v>43669</v>
+        <v>43710</v>
       </c>
       <c r="H13" s="8">
         <f>H11+20</f>
@@ -5659,11 +5863,11 @@
       </c>
       <c r="F15" s="2">
         <f ca="1">F13+2</f>
-        <v>43668</v>
+        <v>43709</v>
       </c>
       <c r="G15" s="2">
         <f ca="1">F15+3</f>
-        <v>43671</v>
+        <v>43712</v>
       </c>
       <c r="H15" s="8">
         <f>H13+20</f>
@@ -5750,11 +5954,11 @@
       </c>
       <c r="F17" s="2">
         <f ca="1">F15+2</f>
-        <v>43670</v>
+        <v>43711</v>
       </c>
       <c r="G17" s="2">
         <f ca="1">F17+3</f>
-        <v>43673</v>
+        <v>43714</v>
       </c>
       <c r="H17" s="8">
         <f>H15+20</f>
@@ -5840,11 +6044,11 @@
       </c>
       <c r="F19" s="2">
         <f ca="1">F17+2</f>
-        <v>43672</v>
+        <v>43713</v>
       </c>
       <c r="G19" s="2">
         <f ca="1">F19+3</f>
-        <v>43675</v>
+        <v>43716</v>
       </c>
       <c r="H19" s="8">
         <f>H17+20</f>
@@ -5932,11 +6136,11 @@
       </c>
       <c r="F21" s="2">
         <f ca="1">F19+2</f>
-        <v>43674</v>
+        <v>43715</v>
       </c>
       <c r="G21" s="2">
         <f ca="1">F21+3</f>
-        <v>43677</v>
+        <v>43718</v>
       </c>
       <c r="H21" s="8">
         <f>H19+20</f>
@@ -6023,11 +6227,11 @@
       </c>
       <c r="F23" s="2">
         <f ca="1">F21+2</f>
-        <v>43676</v>
+        <v>43717</v>
       </c>
       <c r="G23" s="2">
         <f ca="1">F23+3</f>
-        <v>43679</v>
+        <v>43720</v>
       </c>
       <c r="H23" s="8">
         <f>H21+20</f>
@@ -6115,11 +6319,11 @@
       </c>
       <c r="F25" s="2">
         <f t="shared" ref="F25" ca="1" si="0">F23+2</f>
-        <v>43678</v>
+        <v>43719</v>
       </c>
       <c r="G25" s="2">
         <f ca="1">F25+3</f>
-        <v>43681</v>
+        <v>43722</v>
       </c>
       <c r="H25" s="8">
         <f>H23+20</f>

</xml_diff>